<commit_message>
perbaikan prometheus dan grafana
</commit_message>
<xml_diff>
--- a/data/user-data.xlsx
+++ b/data/user-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abdul Aziz\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79E7EC08-3299-4CE3-B43B-ED15F532B102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4178B4B-EB9E-478D-A647-9EC4F392200D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7572" yWindow="4116" windowWidth="23040" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4392" yWindow="3708" windowWidth="23040" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="127">
   <si>
     <t>nip</t>
   </si>
@@ -58,27 +58,9 @@
     <t>TlQAELANAAAKAU5GVBCmDQAACgFORlIlnA0ZAAFoAfwB/AEAAP+wAQEfAAAAB/wgBxGBoAdGC4aStsALTgiSfBGBBjgNlpslQRBBBIwGMgEFMAyXCG1hBEsOmSJ5ARA4B5QdeoESQQiRmwliDEUGoYZKIghOEZIjYkIUHASVJmmiDFUFoaedghUlBo1dqaIDQhaHo74CEEcCmE7iggQ0Mowb6aIFPGCQO/5iBTVylCESoxQnB4VLQqMCKBiRq0KjDkUDkipG4wU9E5enhYMIRQqar4njBjcNlJmSwwIXVYGoxeMNTgiQiQWEBCEKfJ4exAtOCJyXPWQSSAaJlnEEEEECk5V1hAlKC4uPsaQMPgWDBoABAwIVBP9v/////wHx////////AwgZAgBR////AAFVAwhVBQRBAf8f////BwYTBQKFCAk4Bf8v////AAJhCAkW////////BAYmCggnCQLEAQMzB/8vCgtLCAaSA/8f////AgNZBgp1DgsTCQVR/wX2BgjFCxY3EA1TDBQYDghVB/9P////FBUrEAmDCAY5Cg5xCv8f/////xLzDgtX/////wX6CRQ1DxMiCAcZChJSHBRjFguxE/8fDQUrCRBBERUSFxFBEw9BDQk1CxSFGBMi/w/xEAsZFBVh/xz4FA5SCgwz/////////w3yDxUTFxgxCw4jEv9fGRs3FhB1FxgTE/8/EQkYFBaBEAsqFBl0GxoWFxUhEQscFhshHhpVGBUx/xPxFRczGv8v////FA43/xzxHRtEGhaU/xjyFxtUHv8f////FhkUEh2xHx5E/xr0GRIY////////HRszGxQWHP8/////Hx5EGhYWGx1EH/8f////HhsUHf9P////////AQQoBYMFAAcABAAA8CMPiSAISQmKjq6AC04Ik3wVAQY6DJabGcEPRwWOCDZhBTINmgxp4QROD50ihWEQPgeWHIbhEkEIk5n9AQxIBqN0CgIDLQ6X9BpiASMHlYE+ogdPEpQsaqIUFgWVJ3UCDVQFpKmNIhUoBpCksqIPSQKdWrUiA0UTiEnqQgQ1Ko4h6SIGPFGSNApDBTtalioVIwYjM5kgIgMVJgiKqTKDDkUClVhSYwItHI4wUiMGNgyYqn0jCEUJmrGFowY4DZSnuaMNUQiRivnjAx8MfZ8WhAtNCJyZNeQRSgiLlWWkD0EEl5RpBAlJC4uNrSQMPgaEj95EEBcGfaQBAwgYAv9P/////wHx////////AwgZAgBR////AAFFAwhEBP8fAf8f////BggoBQBxCAs5Bf8v////AgMVCAsWCf9f////BAMnDA0oCAJiA/8vB/8vDA1bCAaSA/8f////BAM4BgxlDRQvCwVRCv8fBQFeCxInEP9fCRAVF/+P/////wX1CQUmAwjlDRk3EhBTDhYZDwZiB/9f////FhQvEgtzCAYoDA9xDP8f////FRY4DwhUCAcaDBVjHhZkEg2R////CglVCxIyERciF/8fEAknCxJRExgjFBPxERASCQt1DRZ1HBdD/xHyCxJhFBjxGBz/FxP/Eg3/Fhv//x74Fg9jDA5D////DQ8kFf9vGx04GRJ1/////xHxExg0HP8vGhwVFxFDFA37FhmRFA35FhtzIBxVGhgRGA0bGR0RIBxEFxEyDRZTFR6BHx00HBmD/xfyGh1EIP8f////GRsUFR/BIf9PIBpBGxUY/////yL1Hx0jHRYWHv8v/yLzISAzHBkVHR9DIf8f////IB0UH/8/Iv8f////HR9D/////////yHx4RcQjYAISwutjKLACk0JspoZwQ9HA7EQbWEFShLDIYLhEDIHsx2C4RI+B66W+kELOQm9fEICB0cZuAtlIhYPBK8kgUINTgW7p5FCFSYHqaC1Qg87BLhZvuIDMyCtqBFDDjsCty4iAxUlB5umeUMIPgm3qLmjDU0Js5X94wMgCpehFkQLSQi4nDnEEUgIrphtxA8/BLGVcSQJSAqmj8pkDDIGlBQBAgYZA/+P/////wHx////////AgYZAwCBAf8f////BAYpAwCBBgcW////////AAKICAn5BgByAv8vBf8fCAn7BgSRAv8f////AwEZBAp1CQ8vB/9P/wP2AQbkCQ0/DP8//w7/Cgv/BAX/////DQ//DAdjBgQpCgtxBQhP////DhA7CwZlBgQYCg5jEw1vDwnx/////wP6Bw0/DxH/CQv/Dv//EBL/Dwf//xD4DQvzCv8/////DAn/DRD/EhH/////DQv3DhOBFBJEEQ///wz/DxL/Ff//////DxD0DhSxFhVE/xH/EA4Y////////FBIzEA1PE/8/////FhJBEQ//EhREFv8f////FRIUFP9P////////jR0KkcAIRgqvi6LACk0JspoRYQ9IBLITceEFShHFIJJBETEHsxySYRM+B66U7gELOAm+dzpiBkEZuhtxIhYTBK+kecIUJgWqKJGiDU8Fu6Gp4g47BLlWvqIDNB2sJu2iBjhFsjgBYwQaRbIoDgMGGlKzqBFDDjQCtzAWQwUjVLMkIgMGITezDiZDFQgGmSRpwwENJKWPacMHEgi2qK1DDUsItaEK5ApECLidKQQRRwmvlV1EDz8GtJJlpAhECaaLvgQMMwWck+JEEBgEmFwBAQYZA/9/////////////////AgYaAwCBAf8f////BAYpAwBxBgcW/////wD3AQKHCQpJBgOGAv8v/wXyCAr7BgSiAv8f////AwEaBAmFChUvB/9f////AwZlChA/DQz0/xP/CQr/Bf//////Bf9PCP//ExY6CwZVEBX/DQfzBgQpCQthBgQYCRNTGBBfDQrx/////wP6Bw1PDhT/FQ//Dgz/Bwb/ChD//xT//wz/Bw3/DxH/EhQfEQ4fBw1vEBbzCgv/E///GBb/FQf/GhRf/w7/Bw1vDxIRFf//FBHxDw0fEBb0////FhCPCwkz/////////////w7/ERf/Eg3/ChD/Fhr//xT/ChBfExiBGRc0FBX/FRb0ExnBGxpU/xT/FhMY/////xz1GRcjFxAfGP8v/xzzGxpDFBX/FxlDG/8f////GhcVGf9PHP8f////FxlD/////////xvx/x8SgcAHQwltlLagC0wIdn4VYQY3DHydIQEQPQZ0A0UhBTEMggZpQQRKDH0igUEQOQh4HYmBEjUKem4CwgMuDXycDaIMQweE7jFCAScHfItKIgg+EHclaaIMUwWFXamCA0MQbaS6AhBJAn1P6kIENCBzGuniBTxKdzwCQwU0YHokDoMUJQtxqjqDDkEEfCtG4wVAEYBOSqMCMBR3p4mDCEQKgKyNAwc3DXyYkqMCFXJvp73DDU0Idp4exAtPCYCXPSQSRgdylF4kEDgEfZRxRAlHDHaRtYQMOQdrdAEDAhUF/4//////AfH///////8DCRkCAFH///8AAVUDC1oE/y////////8HBiMEAWEJCzgF/y////8CASYJCBUK/2////8EAygOCXcLAsQD/z//B/ISDnkJBpID/y////////8FAlkJC0ENClEEAzkG/38ODBMLCFQLDRUV/3//////CPEIBRYGDMMOFkcQClETFCsQC4MJBjn/DvH///8KCFULEDMPFSIJBxn/EvIbE2MQDJEV/x8KDWILEEERGBEXFEMRDxENCzUME4UYFSIPDRMQDBkTFGH/G/gTDlIH/3////8MDiMS/18ZGjcWEHUXGBMV/z8RCxgTFoH/////DfIPFBMXGDEQDCoTGXQa/x8XFCEUDBwWGiEd/18YFTP/FfEUFzMd/y////8ME2P/G/EcGjQYFnQWGRQSHLEe/08dGEIZEhj///////8cGiMZEzUb/y////8eGkEXFlYaHEQe/x////8dGhQc/0//////////HhCJQAhFB3OQqkALTAd4exHhBTcLe5wZoQ9BBnYJPYEFMQ2ECWnBBE0NgCKJgRA9CHodkcESOAp7nAVCDEcGhmkKQgMtDn/sJaIBJgl/hULCB04PeyZ14gxTBYhbtSIDQw9upbbCD0cCgiDpQgY8QHpK8gIENBx1NhIjBTo7fSkZQwYjJoCqLmMOPgN/L04jBjcMglxWQwIjFnapeSMIRAiCsoWjBjgNfaixYw1OCHifFkQLTQiCmTWkEUUIdZZaxA85BoCVacQIRg13j6kEDDsIbmgBAwgYAv9P/////wHx////////AwgZAgBR////AAFFAwtKBP8f////////BggoBAFRCAsoBf8f////AgMVCAsWCf9f////BAMXGgzICAJiA/8v/wfx/wz6CAaBA/8f////BAMoBv9vDBIvCwVRCv8f/wX1CAtCDf9fCw8WDf9P/////wnxCQUmAwjlDBY3Dw1TExIvDwtzCAYo/w7x////CglFCw8yEBUiCAcZ////GhNkDwyRFhIfEQ0SCQt1DBN1Ff8f/w3yCw9RERci/xXz/xDyCw9hEhTxFP//FRH/Dwv/Exj/DA4k////GhgzFg91F/8fFRFBEgz7ExaR/////xDxERQ0HP8/Egz5ExhzHP9fFxQRFAwbFhkRHP9PFRExDBNT/xrxGxk0/xbzFhgU/xvxHf9PHBVDGA4W////////GxkjGBM2Gv8v////HRlBFxZFGRtEHf8f////HBkUG/9P////////</t>
   </si>
   <si>
-    <t>RUSTY ARI MEI MANALU</t>
-  </si>
-  <si>
-    <t>BTN0003694</t>
-  </si>
-  <si>
     <t>00701</t>
   </si>
   <si>
-    <t>TlQAEAwNAAAKAU5GVBACDQAACgFORlIl+AwZAAFoAfwB/AEAAP+pAQEfAAAAB/UeBytKwBw3BKaQZsAXThCQ5rmgDEkFqCi6IBdBEI9lvcARShWVq77AHiYCqd0JoQhLBJPwGqEPTguNEl6BEVQjgCuCYRVQDI57lSETLiWBB6khESoqea7CgRxPAqIo6YESQyp/q+2hF1QCrd8+wghGBoCrjiIYWg2ZPZGiEhg+jGGiogxMBImnvcIaWAqLjcqiFC0tiZveYhZJEovfAWMMQAiQmgljG1QIg5UqQxlTBofiNuMIOwmO6FqDD1EIhYKSIxdVD3WNoqMaQAp39bnDEEcPdgZoAQUDFwH/X/////////////8A9QwDEgQCQwQHRQsP9gb/L////w4JVQT/L/8B8gD/fwL/T////wMMJQgHQQD/H////xMM5gMBdQIHJhIPx////////wMIIgsP8QYCZf8E8QoLHw8GGAcEJAMJURANFAoIIf8D9f8O8QYIkQMJcg4QMQ0LPw4N/xIP/wYI/wMK/wX/b////xMQZw4DYRES8g8LTwgKQw4QUgMFXQz/bxARLw0JUQsS9BYZdf////8G9w4MJ/8T8RgVMxQNQhoW/xIL/w0O/xUU//8P9AYNwhEU9hoWYg4MFv///xcYJBUQQREN8hATRRUbFBoSFQ0QExMXQhgbFBoUEREa9B3/fxn/Hw8SchMMJ/////8c9BgVIhUTFBf/Lxz/LxsaMhYaFP///////w8SURUbEh3/PxkWRBIUYRoVJBj/Pxz/H/8d8RUYMv////////8b8Rv/H////xkacxQVVQEEYF2iEAEHALSCE////wAEAAD/HixWAB03BKmMWmAXTRKP6LHADEgFqayygB4mAqsqwmAXRQ6SY8VAEUsSmN79AAlOBJf1DuEPUgyPHFYBEkkmgW2JYRIlLX4piqEVUQuTG6XBESEve6+yIRxQAqao3UEXUAOtLPUBE0cchd8yIglLBYNffWIQIByCXX0iESo4hK1+whdbDJxhrkIMTQSKqbViGlgLjqfS4hVMF4zf9cIMQQeQnP3iGlUIh5MiAxlSB4nhKiMJPQeM7E7jD1EIhn+KgxZWD3WQmiMaQwp4+qkjEUQOd2gBAwQYAf9v/////////////wD2AwRjBQJCBQc1Cw/2Bv8f////AP8f////FAzHBAGGDQpWBf8vAf8/AAyBBgJD////BAwkCAdBAgcWEw/H////////DAhzEA/yBgJl/wXxCQsfDwYoBwE4BAph/wfzCAQXCg0iDgsvDQ4UCQghAQSGDP9/DhH/Dwb/Bwn/Cg3/A/9/////FBJoDQRhCgMdDP9vEhEvDglCFREfDwI6Cwr0DRJCCxD/ExlW/////wb3Ew//Bw7/DRH/HRr/ExD/Bw7/DRX/Gxr/DQwo/xTxGBVEEQ7y////DwtfEBX3FhkhDQwW////FxgUFRJBDhIUFBhBGx1VGhEvEBr0Hf9vGf8fEw4jFAwX/////xz0GBUiFRQUF/8v/xzzGxpCFhoV////////DxNhG/8/Hf8/GRZUEBXyGhU1GBdFHP8f/x3xFRhD/////////xvxHP8f////GRpzFRtR/hmJXmAXRhey6Z4gDTkHwF3eABE9GbYr3WAXOxK13gHhCEwCsuwSIRBLFLAZXoERUTCjKKbhFVMLtq2mIRxNA8il2WEXUgTJKeohEz8jpt8+wghIBaFTXkIRMV2jrHbCF1sMvV+qYgxOBKiptYIaVg2ui86CFCs/q6jNYhZBGK+dCUMbVAmlkSbjGFQHp94uQwk8B6/vVqMPTQmogJZjF1YPlYyiwxpACpb4ucMQSA6ZLAH/////////A/MFAlQAAiQKBJH///////8EAVT///8AA0IGBTEHBlUC/y8A/z//CPEBBRYMC9f///////8DBjIKC0EEAWX/AvEKDCULBBgFAiMDB1ENChMLBkEAA3UICWEA/x////8PDWcJA2ED/18I/28NESYKB0EQDCMLBDoGByMJDUEKDDUO/0//////BPcOCxUEBtUKDTUQFRIJCCf/D/ETETMMClH///8LBkQMEBQVFFEJ/x////8SEyQRDUEMChINEUETFhQVDhQJDWMPE0EWGFYQDBIPCCf/////F/QTESIRDRMS/y8XFiMYFUEMFRT///////8LDlEW/y8Y/z8UDkUMECEVESUT/z8X/x//GPERE0L/////////FvEW/x////8UFXMQEVa4HIROABdGGrLsjqANNQjBLeHAFzsPuWDmgBBAFrXf9UAJSgK0BAKBECUYsSBeIRJFNqKunsEbSgLKJapBFk0KuqPRARdOBsYp9mETPhyo3zIiCUwFo1ti4hAfTqKsYkIXWgjBWGaCERxRpV2GYg8wCaKolgIeGQyorKkCGlYNsWK6AgxPBKmqxeIVPxyw3doiDTMGraD5ohpVCqiMFmMYTwmp3x7DCUEHrvNK4w9PCad8jsMWVxCWjZojGkMKmPutYxFFDphQAf////////8C8wUDVQADNQoEof///////wgGVQP/LwD/P/8H8QQBVf///wIHNgYFQQEFFgwL1////////wgGMwsEJv8D8QACUgoMNgsEKAUAOAIIUQD/L////xANOAkCYQkOGAoGQQAChQcQdAgCFAcQYw0TJQoGQRMOFAsESgYINAkNQgoPRhL/X/////8E9w8LFgQK1AkOgRYYRAkHKBARURYTQw4KYg8MIQQK1AkNhhMYIxQLFgQG1gwTFBsYhQf/P/////8V9BENNQn/HxD/PxUWFBMNMf///wsGVQ8UIhgXYQoNExEWMRkYUhQOQg8TFBj/Xxf/HxIGJxEHFxD/T/8a9BYTIRMNFBEVQv8a8xkYQhQYFf///////wsSYRkbM////xcUVQ8TUhgTNRYVRRr/H/8b8RMWQxD/j/////8Z8Rr/H////xcYcxMZUdUdK0KgHDcFiJJeoBdNDnUoukAXQQx2Z8HAEUcSeOTFQAxEBIjdCaEISgZ47hLhD0wLcwtagRE5HWiGgqETJxxnK4phFVEJdgmpIREpJGOtvmEcTgKEJ+mBEkMia631wRdTA43ePsIISgdqXHrCDzkMbqqKIhhZDX1CkkITGiR2YaqCDEwFcqa5ohpXCXPaxQISFxpsjMZCFCo+b5zaIhZFEnLfAWMMPQh3mglDG1AIapYqAxlOB3DmWoMPTQhthpZDF1APX/WioxA4DWNcAQsCZwH/X/////////////8A9QsCEgMEQwsJFQP/LwEAJ////wT/T////wILJQcGQQMGRQoOlgX/L////wQGJg8O1////////wIHIgoOQQUEZf8D8QgKEg7/HwYDJAL/XwcDFQIJYQ0RJQwKMRAMFAgHEQECdQsNYQwRIw8OQgQHkgIIgQD/b////xMQZw0CYREPIw4KQgcIQw0QUgIAXQv/bxARJwwJUQoPJRL/T/////8F9xIOFQUM0w0RghQX8Q0LJ/8T8RkWMxUMQhQS9Q8MIg0QdBYVEf8O9AUMwg8UHxoXYg0LFv///xgZJBYQQREV/xsa/xcS/w8M/xEMEg0QdBYbFBoUHxEQExMYQhn/HxoVERQa9Bz/b////w4SchMLJ////////xkWIhYTFBj/L/8b8xwUPxYbEhz/L/8X9BIUbxoWJBn/P/////8c8Rv/H/////8a8hQW9P8dK0rAHDgEi49WQBdNEHXmuYAMSQWKKcJgF0EKemTFQBFJD3zd/QAJTAV88wpBEEsNdRpSIRJTH2l7egETLSFnLI7BFU8IfBahoREyI2avskEcTgKIrOlhF1MDkCv1IRNHE3DeMkIJSwVtWn0CESk1ca1+whdaC4FdgoIPKwhvqLFCGlcKdWG2IgxMBnWnzsIVSxVy3vXCDD0IeJr94hpTCG6TGqMYUwhz4R7DCUEHc+hO4w9OB2+BiuMWUxBgkJpDGkAKZPWiAxE4D2NcAQsDeAH/b/////////////8A9gsDIwQCQgQGNQoOhgX/H////wsJFgT/LwEAOP///wL/P////wMLJAcGQQIGFhEO1////////wMHMwoOQgUCZQQBFQgKEg4FKAYBOAMJYQUHgQMAfgkMIg0KMRANJAgHIQMAbgsMcQ0PHw7/LwYHQggJEgD/f////xIQaAwDYQMAXQv/bxAPLw0JQRQPHw4COgoJFAwQQgoRJhP/X/////8F9xMR/wUN/wwU/xoZ/wwLKP8S8RcURA8N8hMOJgUN0wwPnxwVcQwLFv///xYXFBQQQf///w4KUxEUJxUYIQ0QFBIXQRocVRkPLw8a9xn/Txj/HxMRIRILF/////8b9BcUIhQQFBb/LxsaNBwZQhUZFf///////w4TYRcaIxz/P/8V9BEUUhkUNRf/Txv/H/8c8RQXQ/////////8a8Rr/H/////8Z8w8U9Q==</t>
-  </si>
-  <si>
-    <t>EKO RESTIOWATI</t>
-  </si>
-  <si>
-    <t>BTN0004670</t>
-  </si>
-  <si>
-    <t>TlQAELUMAAAKAU5GVBCrDAAACgFORlIloQwZAAFoAfwB/AEAAP+aAQEfAAAAB/8gB3oVwA0pA4h+FeAUMwKE9H7ABjMGeffJQAtZBIQG3qAWVQaAEC1BHTsKhPtiYQ9ZA4Z1aYEJVwKK9aZhBE4DjGjRwQETBJIT3qEWVgiNcA0iA0oGmRodohxRB4ZrKsIFWAiccT7CCk4EoQpC4hBYCY2UcWIYUgaI8IKCBUQFoP+yQgxcC5mIwiISVAuOJNViHR4DifL2YgdaBpOHRaMRWAqIaEmjA0wDje+lYwhVBYD2+sMKVgd/aQEkCFAFfZQexBJTDIFiIqQCLwSNg4JkEEsbfPnlpAtFDHfqBiUHTQl1BoAB////////AQoeAwJRAP8f/////wT2BgOUAQMTCP9//////wDxBAYlBwhVAv8/AAFUBQoXDwazAAF2/////wz3CgRxAf+P////Cg83DghhBwMVAQST/wL3AwRTBg8YDghxBg0UCwk/////Agdx/////wL/CAv/Ef//EBY8Dw5DBgQ3BQxx/wn/CAc0DRElF/+v/xT0EApRBAV3/////wvyCAdFDhInEf8vDQgmBwZ2DxIUGBGhFBMjEg4xBwaHBAq0CgU7DP9fFBstEw9RDhUUF/9f/wv1DQcnExsZGBVhEQ5EBg+jDg9DChCF/xb0GBJh/xv+ExBiDP9P////Fhk4GBdR/xH0DRJxEhNEEBSa/xv1GRhS////CxWhEhglHP9fFhkjGhwx/xf1FRJWGx0THv9vGhgTEhaVHBcnGBI5GR0UHv9/EhaVFP/v////HRky////CxflGh4pH/9/GRI9G/8//////x7y/////x/xHBqXGR1iHv8f/////xz3GhlUAAQABwAEAAD/H3gVQA0pBIh9FWAUMwKH9HpABzYFfPjFwAtZBIYF5iAXVQWCFjnBHTsKhf1a4Q9bBIh1cQEJVwOO9aLhBFQDjxXmIRdZCI5sEcICTAabHykCHVMIh2w2QgVXCJ1xRkIKTwSkCkZiEVgKj5JlIhhXBovxesIFQwWiAa7CDFwKmIW6ohFVC5Ax4cIdHQOL9O6iB1oGloQ9AxFUC4xkVSMDUgOQ8Z3jCFgFg/vuQwtaCYJpDaQHUgR/kRJEElMNg2UuJAIpBI98dsQPShp+/d0kDEIOeOv2pAdPCXZ0Af///////wEGGgMCQQD/H/////8E9gYDkwEDEwf/f/////8A8QQGJQcIRQL/PwABQwUJGA4GxAABdv////8L9gkEcQH/f////wkOSA0HcQIDhQEElP///wMEQwYOGA0IcQYNFwwKU////wIHgRMPIw4NVAYESAULcf////8I8w0MQhb/nxMaPg8JQQQFdv////8K8ggHVQ0ROBD/PxAIFwcGdw4RJRcUpRMSJBENQgcGiAQJxQYJYwv/TxMaHRIOUQ0UFRb/X/8K9QwGNxIVFBcUYRANVQYOtA0OVAkPlf8a+hURQf8a/hIPYQv/P////xUYORcWUf8Q9Q0RUREOSBITSf8a9RgXUf///woQlRQXFBkbZRUYExkbIRYKTRQRVhocJB0ZYRYXcxEVpRsWJhQXchgdFh7/XxEVpQ//3////xwYQv///woW5RkeKP///xkYRBoTTv////8d8v////8e8RsYlhUcsh3/H/////8b+BkYVf8Z9H7gBjEClvjFYAtXA6kF4qAWVAemDzVhHTsKqv9ewQ9YBa1zbSEJUwGz9KIBBVIDthjmYRdXCrRwGaICRwi5GR2iHFQIrGkyQgVUCcENRsIRVAy6kGXiF1YIsQSu4gxZDMODvmIRTg249e4iCFUHvYNBQxFYDrJnVSMDTwO086GDCFcFqPz24wpbC6ZpAUQIUASikCKkElQPpICKZBBMH6D91kQLPwyZ6woFB00JlCwBAQQ3Bf9/////////AgQlBQZVAP8/////Awf3CwSzAP9f/////wn/BwT/Av//////Bws3DQWhAAF1/wLz////Af9fBA0bDwaxBA0aCghD////AAVx/wzzCwRDAQKXAwnx////AAajCg8pEf+v/xX+DAdRAgN//////wjyBgVFBA1GDxFn/w7zDQozBQSHBwxBBAdjCf9f/xX9EAuRDhUZEg9hCgVrBAujDQQaCww1/xD0Ew+RDhMYEhFR/wr2BQ2xDQ5ECwmN/xX1ExJS////CAqnDxIVGP/PFRMzFP8/EQheDw1WFRYTFxRRERJzDRCV/xH3EhA1ExYUF/9vDRCVCf/v////FhMyEw09Ff8//////xfx/////xjx/xT2ExZRF/8f////////FBNU6Bt9GWATNAKk9HqABzYCmvjF4AtYA6sG5gAXVAenAFphEFwFr3F5gQhSAbbwnqEFTwO4Ge7hF1UKs2wdAgJHB7oeLQIdUgirbD7iBFMJwXNOwglJBMsPTiISUQ27jVVCF1AJtfNu4gY8BscCrkINWQvDgrbCEE8MuvjioghYCMCDQYMQVQ+1ZGHDAk8DtPWZIwlTBqsA8mMLUw2paRGkB1IEo4sSZBJREKV7fsQPSCCiA9LkCzsQm+z6hAdPCJVEAf////////8D/wQC/wAC8wX/f////////wMEJQUGRQH/P/8A//8H+AwExAEAb////wcMSAsFcQEChQAD9P///wECdAQPGwsGcQULFwoIU////wEChf8N8wwEVAIDmP8J8f////8G8wsKQhP/n/8X/g0HQQP/f/////8I8gYFVQsOMxP/fw4GFwUEdxAPVRETVf8S9xALQwUEiAcNUQQHY/8J9P///xIMgQsRFRQTlf8K8wYEdxASFBQRYQsFWwQMtA8EGwwNRf8X+hIRQRAVGRQTUf8O9QsPUREQNAwJfP8X9RUUUf///wgOlREUFBr/zxcVMxb/LxMKSxESURcYJBoWURMUcxIJXv8T9hEUchUZFhr/XxQSNQ3/3////xgVQhYVRBIXlP////8Z8v////8a8f8V9hcYYhn/H////////xYVVf8b9slAC1QFagbewBZRBmkPLUEdOQtt+l6hD1cDbXVtQQlWBHH1psEETgRyE+YhF1cJc24JIgNOBX4bGaIcUwhtbSrCBVcHfnE6wgpLBIIKQkIRVwlylm1CGFUHcO55AgU/BYL+skIMWwt8h74CElMKdPH2YgdYBniJRYMRVglvZU1jA1EEdO+lYwhTBmj0+sMKUwZsaQFECE4GZZcixBJRC2hkKkQCLAd1iIaEEEgWZ/TppAs/CmDsBuUGSgpgRAEBAyUEBVX///////8CBvcLA7P/////////CP8GA/8B//////8GCzcKBWEEABX/AfP///8AAVMDCxgKBXEDChYH/z//////BPH/DPMLCkMDATcCCPH/////BfMKCUIS/6//Fv4MBlEBAn//////B/IFBEUKDicQDXIJBSYEA3YLDxQOEET/D/MOCjEEA4cBBrQDBmMI/1//Fv0PC1EKEBUS/2//B/UJBCcPFhkTEGENClQDC6MKC0MGDIX/EfQTDmERFDgTElH/DfUJDnEOD0QM/5//FvUUE1L///8HDaYQExUaF8URFCMVFzH/EvUQDlYWGBMZ/28VExMOEZUXEicTDjkUGBQZ/38OEZX///////8YFDL///8HEuUVGSka/38UETkW/z//////GfL///////8aFRcUGGIZ/x//////F/cVFFT/GffF4AtUBW0F5kAXTwVr/1ohEFgDcHZ1wQhWBHX1nkEFUgR1FOqBF1YJdXAZwgJMBYMcKeIcUAhtbTZiBVcIgHNGYgpPBIcKSsIRUwh2k2HiF1UGdO91YgU/BIUArqIMWwp8hLqCEVQKd/PuwgdXBnuGPQMRVwlyYlkDA1AEd/GZAwlWBWz38kMLVwduag3EB08FZ5QWZBJRDGqAegQQSRZp+tkEDEIMYuv+ZAdKCmIsAQECJQMERf////////8F+AoCxP///////wUKSAkDcf8A9f8B9P///wABQwINGwkEcQIJFwgGU/////8D8f8L8woJVAIBSP8H8f////8E8wgMJBH/n/8V/gsFQQH/f/////8G8gQDVQkNOAz/LwgENwMCdwoNJRIPpf8O9BINpAMCiAELwQIFYwf/T/8V/Q4KUQkPFRH/X/8G9AgDJg4QFBIPYQwJVQIKtAkKVAULlf8V+RANQRATORIRUf8M9QQNwQ0ORAsHjP8V9RMSUf///wYMlQ8SFBT/bxATExT/LxEGTQ8NVhUWJBcUYREScw0Qpf8R9g8SchMXFhj/Xw0QpQf/7////xYTQhMSRxX/T/////8X8v////8Y8f8U9hMWYhf/H////////xQTVQ==</t>
-  </si>
-  <si>
     <t>arian</t>
   </si>
   <si>
@@ -121,15 +103,6 @@
     <t>TlQAEFwQAAAKAU5GVBBSEAAACgFORlIlSBAZAAFoAfwB/AEAAP+nAQEfAAAAB/8kB3wKoA4mBIhrMSAMRAqOcWYgEVAIhuyZAApPCYVdwkAHMgd/i9bAGlIJi3T5oBJCCIf0FgEPUwmGABYBEzYJhlpGAQdRAZNkfUEPTgqGf5bhFlYLiloFIgtXBZjnCQIOVAiTYh7CEkYNjQIdIhVUEItgJaIQSQuYlJniG1MIh36qghhTEpFcsWISUQ6b4snCD1AFpHb2IhhCG5LyBqMTSRSREiYjF0okkFBhAwdLBZo9ZgMXKmWKRmlDElMQjCCGgxg+FI1KkgMMVwijKZZDFzsgijuaAxRUEYmlooMdQhOSn0EkG0MShBFGxBhFEoEWekQYSA5/JwGFDkMIiQawAf///////wUCUwcBgf///////wACEwcDggEAM////wULKQYJUgIHFgwJogT/H/8B8v///////wMHFgwJogL/L/////8R/AsIYgcCFf///wUIIQ4KgwYOGAr/PwQDZgL/T/8L8w4KcgcGEf8F8v////8E8gcKRwwYi/8J9wcIMgULUhANYwoIIwX/b/8S+A8OQ////wkHhAoNExQYkw4QMxQcdgwJOgcKYxANEwoLYw8SFBYTZBESJBMOQQ0ISAv/T/8N8woIZw4SFhMUZA8FLP////8b+BUSQhMPFAUR4v8f8hUWIRQMKxAOZP8X9hYaNBMWJRocYRj/fw0QdBYPFxIRJP8f8RkXQRcZJBocFRgTsw4SYRsZIh4WIhMSZBX/H/////8M8xQcdiP/nyMeohoWRBf/LxsdESMcVv8U9hYZFB4iJCEiNB0ZERcSJv8f8////xgMaBQaFiEjsyEjGx4aNRkRGRsgESP/fxwaghYZIh0hMhH/T/////8g9h0bUxsfJv///////yEeE/8i8SMYrh4dIR8gcf///yMYnh4hESD/P////////xweNyL/nwEEI2XDFgAHAAQAAP8nfQ5ADiYEiWo5oAtDCo5xbqAQTweJ741gClEIiF7G4AYxBoGKzkAaUgiLeAFBEkMIiPgOgQ9VCIgBFqETNgmGWU7BBlEBlmOJwQ5WCIl8kmEWVguK6v1hDloHk1kRwgpWBZsIFcIVVg+OYCZiEkYNkF8tYhBLCpuQjYIbVQeLe6oCGFUTk+a94g9OBaVavQISVAudc/KiF08alff6AhRNFZQYIqMXSyKRTXHDBkkGmidyQxctT4tFdSMSVRCNNHajFihZiR+O4xhEDY6kmkMdRxKTSp7jC1cHpCeiYxc5GIs4quMTVQ6KotGDHSUgip3qQx0lIIelNWQaPBSFDFYkGUUSgxSChBhJDoEkCaUOQgiL1AH///////8FAmQKAbH///////8AAhMHA4EBADT///8FCDcGCVICBxYMBLH/////AfH///////8DBxcNCaMC/z//////EfwLCHMHAhX///8ICxQMCkIGDxkKCTUEA3YC/1//C/QPCoIGAhf/BfP/////BPMHClcNGIv/CfcDB4MIDiYQDFIKCCQF/3//EvkOD0QOEDITGGINCSoKBiT///8JB4QKDBITGIIREhQUDzEKC2QF/68QDBMKC2QOEhUWFHQYDCIKCFcPEhYUE1MOBRz/////HPgVEkIUDhQFEeL/HfMVFjIUFhUaHlEYDWgQDzIeEyEQD1T/FfQWGjMWDxgSETT/HfEXGiIVGxUaHhYTFFMOEmIcGTMgFjMOFZIR/1//////CfsTHmYm/48fJhsbFhUXETj/HPEmHkb/FPMWGxQgJSQlICMaFkUXETgZHxEjJSUfGSEXETj/HfQR/0////8hI/YcGUT///8YDWgTGhYkJsIjJhsgGkUZERkcIS8m/38eGpIWGzMfJEMd////////Iv8mHP8XIS////////8jHDEcIiP/////JfMkIBP///8lJiogHzIj/x////8mGJ4gJCIj/z////////8eICcl/5/rIGomwAs6BqtkaoAQSQqp7plAClAJpF3S4AYyB5SJ0kAaUAit+hJhD1MLqXgS4RI3C6h6GuESHguoXFqhBk8CtWGFwQ5SC616lqEWUg2x7P1BDlcJtVgR4gpWBboHHaIVUxK2j5WiG1IKrHSqAhhRFbjmtuIPRAi9WL0CElAQufrtwhNFGLRp+mIXQCK1HCLjF0orryBZAxcjZ6tReeMGRQe5RHkjElQUtJ+aYx1CD6pHouMLVAnHNrIDFFMSryK9Qxc7FaWiPQQbORadEEbkGEQWmBGChBhFE5ssDcUOPAqhgAH/////////AfMFAnICABP/////BPIGBVQBBRULA7H/////APL///////8CBRUMCKIB/y//////DvwKBmIGDRkJCDQCAFcBBEEFARX/BPL/CvQHCRIFARUGBBP/CvMLCUL/////A/IFCUcMFov/CPcCBYMHCiIQC5MJByME/2//D/gNC0ENEUkQFmIMCDoJBzT///8IBYQJCxMQFoMODyQRC0QJB3gK/08NBCz/////GPQTD0IRDRQK/48OGCITEiEPESIXGWEWDGgLDWEZECILCpcNE0QSFzQTFR8XGSUQEVMND2ESERQND3L/GPEUFxEcFV8aEiMTDxMOGFEbH/8aEf8SFP//GP//////DPMQGWYf/58fGVb/EfQSFS8aHiQO/0//////HPYbFGH///8WDGgQFxYdH7Mf/38ZF4ISFT8bHTIdHxv/GvMVFPQY/28bGBb///////8dGhP/HvEfGasaGyEYHHH///8f/58aHREc/z//////FvkZHToe/5/KInQqYAsyB6tvbkAQTgmr8YnACk8IqIbGABpQCK5m3mAGLAaW/AYhEFEKqWZiYQZLAbdhkYEOUwqudpLhFU4Mse71oQ5YCbQMGUIWUhG3Vx2CClEFu1w+YhE0DbZcRiIQLgu4jIlCG1EKr+qmQhBCCrxvqmIXTBa6V82CEUsNuvvtIhRAGbVk+sIWKx62HiZjGEUjrzhqwxYoaqtOhYMGQQe4QInjEVUTtZyKAx0wDasZnmMZQAqoRbKDC1IIxyXBgxc/FKSfwQMdLRKnNMoDFFMPr6U1RBo6F50MTgQZRReZD47kGEUTnSEdJQ89C6GYAf///////wEFSQIEIgIAFP///wMIKQUGQgEFFgkEsf///wD/LwH/L/////8O/AgFcv////8A8gIHGQb/PwgMWQcGNQIAaQEDQv///wQCMgUHVwv/j/8G9wIFgwgKJgkLIQcFJf8D9/8O9goMRAoNMw8WYgsGKgcDJw4QFBIMUQcIZAP/r////wYCiQkNJQ8Wgg0LFQkBPQoQFRIPYhYLNQkFOQwQFhEPUwoDHP////8Y9BMQQhARMhcaYv8L+A0MMhEMFQr/Tw4YIxMSMRr/Lw8MJAoSMhUXcxMVFRcaFREMJgoQURoSYQoQcw4UQhUXUhkVNBcSMxMOJf8Y8SEdoxcSRRMURBkbIf////8G+wsaJiH/jyEaRhYRsxIVFB0gJA7/T/////8c/xkUQR4fJBsVIhQOOP8Y9P///xYLaBEXJh8hwh4hGh0XNBUUJBn/LxQY//////8e/yEZ/yH/fxoXkhIVMxsfMxscH/////8g8x8dE/8g8iH/rx0bMR7/H////yH/nx0fIh7/P////////xodJyD/n/8lbTXgC0ALc3BqwBBOCG/smSAKTgpt/KkAEiYJbnLCQBEpCHON1qAaUglzdPmAEkEHb/UOYQ9RCG/9KUETNApsWUrhBlEDeWSBAQ9VCWx+koEWVApy5gVCDlYHdloJIgtWBX4CGWIVUw5xYSJiEkUMc2AlohBIC4CTlcIbUgZwf6pCGE8Qdl21QhJRC3/gzaIPUAWIe/oiGDkVeO8GwxNCEXcPJkMXSRt3Ul1DB0wGgiFqIxcrXXBIbUMSUA5xTYZDDFMGhSGKoxhBEHOnooMdQRV8Oa7jE1QMcCmtAxdAEnSb9qMdIjxwkUEEGx0ScBBSBBlEE3AZdiQYRgxvJwWlDkMHeLwB/////////wHzBwJyAP8/////BQMiBAkhAQcVDQmi/////wDyBQYTCgRhAAFS////AgA1AQMhBQYSCgdRAf8v/////xH8CwhjBwQSA/8/BQgiDwqDBgsUCg00CQJFAQRB/wvzDwpyBwYi/wXz/////wLyBwpHDRiL/wn3AgeDCA4nEAxjCggjBf9v/xL4Dg9DDhBDFBt2DQk6Agqz////CQeECgwTFBiTERIkEw9BDAhIC/9PEAwTCgtjDhIUFhNk/wzzCghnDxIWExRkDgUs/////xz4FRJCDw5EBRHi/xz2FRYhFA0rEA9kERIxFho0ExYlGhthGP9/DBB0Fg4XEhEk/x3xFxoSFxkkHhohGBOzDxJhHRkSHhYiExJkFf8f/////w3zFBt2JP+fIh8hHhYkExeC/xzxJBtW/xT2FhkUHv8v/xj2/w34FBoWIySjISP0HxkhFxEo/x3zEf9P////ICEfHxxjJP9/GxqCFhkiHyIyIiQbHho1GRwSHSFvFx0R////////IRzxHxX/IP//////IyL/////I/8fHh8hICFP////JBuaHh8SIv8f////////Gx43I/+f/yZrPWALQAp1cHJAEE4Gc+6JoApPCHL/oaASJwhscMbAECkGdorKIBpSCXN6AQESQgVx+grhD1IHcgAlwRMzCW1ZVqEGUQN9Y4mhDlMHb3yS4RVVCXLp9cEOWQZ4CBXiFVYNdFkZogpTBIRfKgISUA14XzFCEEoLhJGJYhtTBnN7psIXUQ94XL0CElUKgePB4g9RBYp28qIXQxJ89foiFEwRehYiwxdLG3hOaeMGSweDJ3qDFzg1cUSB4xFVDXNKkuMLVgaHIZIDGUQKdKWWQx1IEX0nuUMXOw91N77jE1QKcqPNQx0lInmc6kMdJSl0ozlkGjoYcQteZBlGEnIYgoQYRwxxJBHlDkMHfMgB/////////wHzCgKhAP8/////BQMyBAkyAQcWDAmy////AP8fBQgTBgQhAf8v////AgBGAQMxBQYSBwkjAf8//////xH8CwhzBwQSAwUiCAsVDApCBg8ZCgk1/wL2BAMi/wvzDAoxBgMT/wXz/////wLyBwpXDhiL/wn3AgeDCA0WDA4hCggjBf9//xL5DQ9EDRAyFBtmDgkqCgYkERIUEw8xCgtkBf+v////CQeEDBAkFBiCEAwTCgtkDRIVFhN0GA4kDAgmDxIWExRTDQUc/////xz4FRJCDw1UBRHi/xz3FRYyGxQhEA9UEhUUFhozExYVGhtRGA5oDBBjFg8YEhE0/xz1FxoiFRkVGhsWFBNTDRJiHBkzHxYzDxWiEf9f/////wn7FBtmJf+PHiUbHxZFFxE4HRxBJRtG/xPzFhkVHyQk////GA5oFBoWJCWyIiT1HhkhFxE4/x30Ef9P////ICL/HBlEIyUaHxo0GREZHCIvJf9/GxqSFhk0HiMzHf///////yH/Hxz/FyAv////////IhzxHiH//////yP/JR//////JCUqHx4xIv//////JRubHx4jI/8v////////Gx8nJP+f</t>
   </si>
   <si>
-    <t>Frisilia</t>
-  </si>
-  <si>
-    <t>BTN0004015</t>
-  </si>
-  <si>
-    <t>TlQAEPIUAAAKAU5GVBDoFAAACgFORlIl3hQZAAFoAfwB/AEAAOOQAQEfAAAAB4AwBxY+IBQQB3KWhcAWEwpxkqVgAwgDhY2mQBYXDHeHwWAUHwh7jN6gBS0HeQj1QBAzC3EL9WAUJAp7i1lBGh0JdAhygRckA3qVduEKQAxxEXaBHQUOb46BQRwYFnSMpSEFQAh/C7KBDjMJfQy24QdDDHuJusELMgh5DcLBHQYGeRPugQo+DXwQ9eETGwp8DvahHBUIeREVIg0oBoGSLiIPHAWCGTnCERQFfhBJwhwSB4CXTqILHAN4jHGiGigGeomOwhMiCX4IlgISIAp/C5oiHBQIfw6pwhRDCn4WxkIRNw57hWpDGS4FfAN2wxcnBX0TrYMZQA56mMFjEE0EhZTVowRBCY8X2QMSPgOFkR2kBUMKiZcphBdCD4MGTiQZIwmFDHEkGgwLihZ+JBY3DIaYrcQUNwWGlvoEDS4Vho0F5QocGYKLHsUOHhaBjR6FEB4RhAZAAgEEEwYCX////////wD/H////wgDQQQFN/////8G/wUN/////wD/HwH/HwgJNAcEIf8A8wEDMQgHMg4GcgL///8G8woNFf///wkTJQ4FYwL//wAHUQkTJw4GUf8E8gP/LwcBFP///wwUFBMJYRQaJRMOQwcEJP8I8QX/HwYOQRASEw8NI/8R8RMMUQP/L////wj/H/8L8REUIxsJgf8F9QAPwRIkHv///xcW8hUQMQr/HwYJUxIkHv8N8f8F9AoQIQUKMQYOURYVEhIPEf8Y9BQTEwwLIf///xkkHv8N8Q8KExAVERobExcW9QYHVwkUQv8Y8hoTMgkMIxH/HxwjGBn/LxIGGQ4WMRAOEgkXfxwjGCQV4Rsc/yQW/w4G/xMa//8d8hoeJAkUQv///xIQExUXLx8kHv///xMMFhj/Lx0gFiEecxcT8wkach4hFB8cIR4jGB//HxYXHxMbQf8o+yAeUhoYEv///yAhNCMckRsTFBQaYyEjFiT/7xYcIRseIh8eEx3/X/8i8ichUSInFColhR8eFB0gYf8o9CclRSEgEv///xkfZiElUSosKiYkmP8S/hkj6Cb/L////yosKi0j8RkfZiEnUSQZLh8j6S3//////x8iVP///ygqFCslUSn///8q8iciFB3/v////y8q/ygi/////////ysmJyUnJSgpLyUiSCr/L////y8mVSYlKisvYS7/H/8t/yYZ/yMs/////////ywjGisvYf////8t/ywlGSv/X/////8u8QAEAAcABAAAfzIcTqAUEQZ0m3VgFhMIc4+iwBUdDXmKwaATFQl6kdKAChkDdZHWAAUtB30R6uAKEAVzCv3gEDMMcgv9ABUeDHsQNUEUIAR4kEnBFSkDeItJwRkeB3SWckEKQQ1yCHIBGCUCe4Z9oRsYFHaNmaEEPwqBibIhCzMIeQu+AQ8zCIIJwmEIRA19EvYBCz0MfA8BYhQdCnoHAiIdFAV8FhGCDxUIhQ8Zgg0oBoKJIsIOJgaDlT5CCx8GeZZJghIWBn0UUUIdEQmGi2UCGikHepSKIhMjCX8EnqIcEwiBBaKCEiALgA2xQhVDC38WzsIROA57j2KDGCsFfgt+QxgnB32ZueMPTQSIErkDGj8LeZLJYwRBCJEW5YMSPQSHkxVEBUMLipcdBBdEDIOYKYQZJBCBCVakGSEKhxOKhBY1C4WYpUQUNQWJjO4kCRoUkpbypAwwE4aFEiUOHhWElxLFDyAQhlgCAgMjBP9v/////wHx////////CwIxAwAh/wDyAf8fCwgyAwYU////AQIhCAkfBwYS////AAdhBgwTDwVi/////wTyDA8l////EQwzDwViBP8fAAdhCRb/EQZB////AwgRDQovCQfxAwISAf8vChT/EQb/BwP/CAv/CQj//wv/DRT/ERD/CAET////DhwWDQofBQYjBxFBEBMkEg8zFRw1FBFECgL1Cw4RCwET/////xXzHA1R/wX1BgxjEiYe////BQxCBxFSFxMiJhLhGhb/FxAyDP8fBwpPEyQYJv/vDwUVDBAxHxki/w/xEhASERcxHB0TGhb/EQofDRVC/xvyHBQyDQ4z////GiT/GBf/EBH/CRT/HyQXGf8vEwYVERgxExETFhT0GiHzJhfhEhMiFxgjISgeJv/vFgr/FBz/HR//Jhj//x7yIBxBDRVC////FA4VFRsxHiIWJyCyFhr/DRyCICQZHxkS////IiBiHA4XG/8vICcYISYuGBovHRwSIiM0JB+BHRQTFRxiIiQWJv/vGB8yHSAyIBw2Hv9vJSMhJyRVJSkULSeVISAkIv8fGSFmIydRLS86KCaH/yr/KSc0Ix4X/////xP+GSTnLihh////LTE5LyShGCGGIylRJhkeISToLv9P////ISNUJSo/KywTLScxIyX//////yv/LCn//////yzzKSofHv/P////LS8pJykjK/8/JykzLP8v////MS5YKCZGJC/C////////KCQqLTFhMP8f/y7yLxkeJzGh////////KCcZLf9f/////zDxtBiQvUAVHgaBBeLAECoFh4zxYAU2BpiUfkELQgeGjKUBBUAGm5KqQRwaCX4MtgEIQgaXirpBCzIIjA66oQ8yBoOMyUEbFQWDFuqBCkAGkpY94gsiA4+OcSIaKgaHD3kiFTsKkhW1whEsBpASrYMZQQeTl71DEE4Cp5HNQwRBCKkXzmMSNwOkkhlkBUUKqpYlZBdCBZ0TkeQVMQafmbYEFDEEoY8NBQ0nFI8gAf///////wUNTQgBYgkNOAgGR/////8A8v////8B9AMEFf///wL/HwEIQQ4HQQYEI/8C9f8G8QoRLv///wD/T/////8M9AkIEwoRHv8E8f8C9AEHcQIDMQEIUQ4LMwoGEQ0OJAsHQQMBFAAJYgD/bwX/H/8M9A0IYgsRHv8E8QYHEQgNIQoHEwgNQw4THhH/7wgJFP////8P+BINsv8P9g4LMwgBKAkMUg8QNxH/7wsIFA0MNv///xQSRA0MaP///wsOdwwSwRYXSxMRmP8K/gsQ6BP/L////xUWNP8Q8QsOZgwUsRELLg4Q6Rf/P////w4PZP////8V9BYSUf///xYTJxIUNA//fxIPSBX/L////xcTZBMQOxIWtv///////3Unj6mAFCQHf43WIBIPA4iI5eAENQWaC+ogFRoEiAvyYBErBYgONQEUIwOJjknBFSsBjoxJIRkjBIsXaQEZGQKNlHKBCkMIiZSWoRsbCYOSncEEPwebj7KBCjMKjwvCgQhECJgPwkEQMQaEi8GhGhUEiBLZIRoNBImP6SEZDgOMFvoBCz4FkRAOIhQbCosPGSITFwiIli1CCyMEkY1hghkrBokQgaIVPAqTE8UiEi0Gk5ixww9NAqgSuQMaQAeTkL3DAz0IqRPWgxI1AqWUFeQERAuqlRnEFkIDnxOdZBYtBp+ZpoQTLAOkk+mkCRkPnpb9ZAwrEZSQBcUJGRWTlxpFECIUk44mxQ4gGYuVJgUTCxWU1AH///////8HA/EBAhX///8AAxEFDvYEAhT/////BPQJCxT///8HBv8FAfH/APH///8FDvUJAlT///8BAxEGE/8OCf8BAP8DB/8FA///B/8RE/8OCf8D//////8KCP8TBv8PEf8TBv8DB///Cv8C/x8EDlEUDPINCzMI////////FvYPBh//AvQEDYESGx7///8CCTIEDmIUEvIbDeESGRgb/+8LAhQJDDEUGPQVEkMJBBUFEf8IB/8K/x//FvMQE/P/Fv8RE/8GCP8P//8GCP8Q////Fv8XE/8YFRH/C/ENDBIOFD8WFxIbFO8OBh8IEf8XGP8bFf8OBf8GE/8NEhEOFE8YHR4b/+8TER8K/1//GvccF7EaHFkYFSIUE/IRFvEaGSYb/+8VFB8X/y8VGGYWHLEgIkodG4f///8eHDQXFlf/////Df4VGechHfH///8eIBUiGbEVGGYWGrQbFR4YGegh//////8YF1ga/z//H/MgHFH///8mIFIcHjMa/28ZHEUeH1L/JvQkHVQdFf8ZIv//I/////8dGSogJWH/////I/8dIf8ZIv////////8dHBogJlH/////JfEiGRogJGH/////I/8dIBQf/1//////JPF1OYfF4AUwCWuJxaAPFApoislACRANb4vaYAsQA2cK4iAHFQNtB+bgDBIIawbqABkTDHIG9cAPMw11DvnACQwNdRAJwQ0WC3QHFaESFQp/ET7BDhYCeoxRYRYjBW4EWSEYGgRvEmahDRQCcI96ARMSB3qShuELNglzj6lBBTwKbI2p4RESBoONsmEOGAp/DrbBBzsPZgjJQQ4iBoML4cEPHg6DCerBCzkLgYrqYQ4fCIUTAcIRGg98GA7CDhsMhxURwgwlC4WTIuITCQVymV6CERsMgZdeIhQVEXeNeUIUIAx1j5JCERUIdQmpghEeEW4LqcIUOwx0BK3CFxgJdImxgg4KDXMMteIMFQtzFMpCETYXaI1ZgxYXCm6KamMZLQlsi2oDHBoHbA2JIxUcDmkKiQMbGQdtComjFyARahOtYxk4EWeWvUMQRgVrltWjBDwJehjdQxI4BWySHYQFPAlxmCmEFzsYdJA5hBogC26MSoQXFQh5CV3EFRQRfwZhRBkgC3UWgiQWLxd/mLHEFDEJeKwC/////wLxBBEW/////////wbxCgcyCQUx/////wHyAwgfEQRxAv8f/wXxCQ4SFAhvCBT0Ef9fAP8f/wLxCQsREAg/A/8f/wHx/yP8DQoy////////ChIWCwkyBQES/wbxEBT/EQT/AAL/AwX/Cw4SEAg/Bf8fAQcyDA8TEwtzB/8f/wbyDxMTDgQRCQcT/wrzCv8fBg0x/x73Eg9C/yP5HA9iDP8fBv8/FhMxEBEVAwkiCw8RCwoTBgxSIxmPEhMjCAXzDhIRExcT/xTy/wT1CBTxGy9O////CwomDw0kHBk/FhMxEA4RChJxFhUhFxQhFy8e/xHx/wj/AxBiFhgRGxdCEBMhBxKCGR3zGhghFQ4TEg04GyUWL//vFBATDhhBEBUhDxZRHRohGxchHh3/JBr/FhL/DBz/HSQfLxvhGBMTFhkvJCX3LxHkFxMUGBohEg81Df9vIx4xHRk/GhkfHB4xIiAhJBvxGRzx////Ih8hIB0hHR4RDf+vIyIiISAhGh0hHh8hJyExLyTvJyo1JiQfGyBBHh8yKCc0LiGRHR8iDSOh/yj0JyJRHxIm////FBr/HSD/Ji7/LyX/Ki4lL//fFBs3HSRPJy4WLyTvGiFBHyIyJiMV/yjxLDIlKi4lIiM0/ynxKy0SMixRIw0+/////zP2KygRMzIjMC5EJiI2Jywh/zP1LSwhKCMVKf8fLTIUNSpxJyMm/yjx/zL0NSphLCgSK/8vJSZWKjBBNf8/MS+Y/xv+JS7YMf8v////Nf8v/y7xJCb2KjJBLxsuJS7p////////Ki00KzNhNjQhNTAxLC0z////////NjIhMDIRLTNBNv8fNzUh/zfxODE4MComMjQx/////zfyNC0VM/8v////ODEnNTIUNP8vMDVDN/8v/////zH1czyJxUAFMQpujMUADxMLZ43JwAgWDG8I6qAHFAZzBepgDRMLbgbqgBkTC3IE+UAQNQ13EA0hDhcKdgkZQRMuC4CJScEVJgVwD0pBDxcCfAJhoRgZB3AQbgEOFgJ1kHaBEhEGfpF6gQs2CHOMmcEEPgtviZ3BFwoLcY2loRESCISNrsENGAl+BcJBCDsRaQXJwQ4iCIQW2gEKLRF2iuYBDhcEhQvpQRAZEoMI7iEMFgmDFRlCDSUKiBcaQg8aC4aTVqIOGQqHmFaiExoLephaQhEWCIKQasIOCQyFCHKiDQoKhJJ9ohMiDniIhqIQFAh6Da0CEh4ScA+xQhU9DHMCtUIYFwp1FbliDRUKcxjKwhE0FmqRVeMVFwtuhWIDGSsLbI9moxsbCW0MiYMbGAduE42jFRoOagqNIxgfEmqYtcMPSAZtE7XDGTsOaJXJQwQ/CX4W6aMSNgZukRUEBTkLdZkhBBc4FXOWKeQZIQ9wmS1EFA0KdolCBBcVDXoCRcQUDA17DGFEFhMQgAVlpBkgC3QUioQWLRV+mKlkFDIIeJf2pAwpFnPQAv////8C8QMPFf////////8F8QYKFAQCEf////8E8QcOFAMAEQ4TJg//XwD/HwIEEgYHEQ4DQgL/H/8B8f8k/AsIMv///////wgNEwoHMQQBEf8F8QoMEg4DMQQBEv8G8QkcGQ0KMwb/H/8F8gj/HwX/PwsjGBENMg0UFAwOIwcBFAYIM/8k+RAN8gn/HwX/PxESEhgOUgIHMgoNIgYIMwUJYiQclxEKIQMEJAoMMhIYFBUPQ/8A9QMOUxMvHv///wn//wv///8k/xwR/woGJQ0QLyQdZhcUIQ4MEgoRQRQWEhgVMxUlFS//7w8DFgcOYxcaEhYYEhIMEgoRQRkvHv8T8QMOdBIYMQ4SMhQXERobJBkYIRwdExoWIRQMExEQLxkfFC//7xUOFBIWMRsfEy8T4RgWEhQaMR0bEy8Z4RYUIhccIRkaExEdgiEeER//LxcNFxAk8iMgMSEdMhoRFhAc8iIhIh8eMhkbIREdgiEtGCUfQSElEi//7xUZMxseIR0cERAk8SMnFiIhER4aEx0gISImEi8l4ycrJCYlEiEdEiAjESgnMy0igSAQH/8k8f8o9CcjQSAQHwX/zy07Ti//zxUfQiEmMictFi8l4iEiISAkMyYjEyQoQSwrETAxTSckFP8p8SouEiwrESQQP/////8q8S4oIf849i4sESgpEf///zMyEjAtMyYnMSgsES4zEjIrMSckFSgqESUmRicwQTQ7+jEvh/8z8jIrMSwoEir/H/8V/iUtxzH/H////zT//zsxqC0mFisyMf8v8SUt2Dv/L////yssIy4zMTg1ETY0/ywuIv////848TcyETAr/ywy/zY6/zsx/zQy8S4zUTj/Hzc2Hzc5/zo7/y00/ys1//858To7KTYr9TU4Ef////858jUuFDP/H////zoxJzY38Tj/LzA2Pzn/L////zsxZDEtKjr/b////////w==</t>
-  </si>
-  <si>
     <t>LIDIA FITRIA NINGSIH</t>
   </si>
   <si>
@@ -208,24 +181,12 @@
     <t>TlQAEM8HAAAKAU5GVBDFBwAACgFORlIluwcZAAFoAfwB/AEAAP+jAQEfAAAAB/8SB5/GoBIpAoSX8WALSwh1lGFBBDoHdphhoRFJCIYWisENTwOCktnhClIHepllghVEBIoTdiIMUQOLHnXiE0YEi5OqIhFHB5AR/iIIUQSVoP6iF0EGgpopwxQqBYWbPoMUKwWEJ8WjFE4GjSX6AxBTBoiZEcQKSAeAo1HEE0sGkAbYAP///////wYDhAH/X/////8D8QQFNgL/b////wEEYwUKGv////8A9P///wgHegQBMQgHNgUCMwH/PwP/PwIBFgQGMgkHNP///wP/X////wsMLwgHJQwP+Ar/XwIFVAMJoQsPHAkHNAP/fwb/LwUDOQgLMgwP+RAH0Q8QJv////8F+QcJVgb/L/////8O9gwJ8gkI/wv///8N/w8H/wkMHwv/P/8O8w8Hcf8R9A8HVA0LNv///////xAKQgkNlw4RUQoJbQ4PlP///////wkOhP////////8P8QAEAAcABAAA/xEcpcASCAOKobpAEioChJjlwApMB3eZUeEDNQV4mFEhEUsJhheSIQ5RA4SRzWEKUgd8mFkiFUgEixJ+ggxQBI4kgWIUQwSMkqKiEEYHkqLuQhdDBYUSBqMITwWXKdEDFU0GkJgBRApFBoUmBmQQUQWKoUFkE0sGkswABwH/Av///////////wD/////BwSEAv9f////AATxBQY1A/9f////AgZRCP9f/////wH0////BwhKBQIxCghnBgMzAgE4BP8/AwIVBQcxCgg0////BABP////CwkhCghVDQ5MDP9vBgVHBAqhDQ98CgYxBQcx/wvxBgU2BwlTDQ9aDAhxCf8f/////w32DAqTDw42/////wb5CAlq/xDzDwhUCQt2////AwzmCw/k////////////DgxDCgurDRBRCg2D/////////w/x/xGftiASKwSemPnAC1AIl5RdQQQ7BZaYXYERTQeoF44BDlMCo5LdAQtVB5+XVQIVSAStEoKiDFMEtiGBQhRGBKyStYIQQge5oPqCF0QEoxMKwwhSBMCZJYMUOgapKtUjFU4GsScKZBBTBqqYEYQKSgeioEWEE0oGscwA////////BgOEAf9f////AANRBAU2Av9v////AQRjBQ8e/////wD0////BgdaBAExBgcWBQIzAf8/A/8/AgEWBAYyCQdE////AwBY////CggiCQdVDA8cC/9fAgVUAwmhCg4cCQVCAwZy////BQRGCApDDA4ZDwfRCP8f/////w32DAkzDg8m/////wX5BwlWCQgUCv8//w30DwfB/xD0DgdUDApG////////DwtCCQyYDRBRCwltDA7E////////CQ2E/////////w7x/xGkruARKwSfl+lAC1AHmJBNwQM1BZiaTeEQTQimF5JBDlQCpZLVgQpSBp+XTaIURwSvEIYCDVIEuCOJohRDBayPqSIQQga6pO4CF0UEpBMOIwlQBMGXFQMUOQasLOVjFUsGs5YBRApIBqUoEsQQUwaroDkkE0oGscwA////////BgOEAf9f////AANRBAU1Av9f/////wH1BQsa/////wD0////BgdKBAExBgcXBQIzAQA4A/8/AgEVBAYxBwtJ////BAAY////CgghCQdFDA4cC/9vBQRHAwmhCgwTCQUxBv8f////BQQ2BghDDA8ZDgfBCP8f/////w32DAkzDw42////AgWpBwxlCQgTCv8//w3zDgu1/xDzDwdUDP8/////AgvmDA+0////////////DgtDCQyYDRBRCQ1z/////////w/x/xCY9YALRglflVLBBDIGYJddgRFGCWwWjuENTQRvktnhCk4IYphdQhVDBnISemIMTwVzHX0iFEUFcpWqIhFGCHOf+qIXRAdrEf4iCE8Fepw+oxQ5Bm4oycMUTQZzJAJEEFIHcpkRxApFB2ijTcQTSQZ0wAD/////AvEDBDYB/1////8AA1IEChr///////////8FBloDADEIBlYEATIA/z8C/z8BABYDBTIIBjT///8C/1////8JCyYHBiULDRgK/18BBFQCCKEJCxQIBjQC/38F/y8EAjkHCTILDRkOBtEH/x//////DPYLCDINDib/////BPkGCFYIBxQJ/z//DPMOBrH/D/QNBlQLCTb///////8OCkIIC5cMD1EKBmwMDZT///////8IDIT/////////DfH/EJfpAAtHCGGZSkEELQZjlk0BEUYJbRiSQQ5OBHGRzYEKSwhkl1HiFEUGcxOCwgxOBXYgiYIURAVzlKaiEEcIdqHuQhdFBm4SAmMITgV8mjJDFDgGcSrZIxVOBnaZBWQKRQdtJQqEEFIFdKI9ZBNJBXjAAP////8C8QMENQH/X////wAEUQb/b////////////wUGSgMAMQUGFwQBMwD/PwL/PwEAFQMFMQYKSf///wP/H////wkHIQgGRQsNHAr/bwQDR/8I8QkLFAgGNAMFMf///wQDNgUHQwsOKgoGcQf/H/////8M9gsIQw4NNv////8E+QYIZwgHJAn/T/8M8w0Ktf8P8w4GVAsJNv///woGbAsOtP///////////w0KQwgLqAwPUQgMg/////////8O8Q==</t>
   </si>
   <si>
-    <t>Rara</t>
-  </si>
-  <si>
-    <t>BTN0000041</t>
-  </si>
-  <si>
-    <t>TlQAEAkKAAAKAU5GVBD/CQAACgFORlIl9QkZAAFoAfwB/AEAAP+pAQEfAAAAB6gdB7E6QAsdBZuwdeAFHBB+vJUADjQIo0Py4AQsCnTGBqEQKwO8yDHhBCAQfcdJQQxJDZDFUaEOHgao1HaBAxQLddSFgQY9CnTJjkETNQKtWrlhCjYGhFbxgQ4cCZ3W+aEJNQaBzxLCDi8KnOEaQgU8DHLKLeIVMgK0XDXiDSwUltBVIhAlCp9baeIOHxWZz6YiDxcLl3CyAgcoCIRQssIXIASr5x6DBiILidAlYxYWB6BZLqMVHgie5U0DDDYFiPn6wwUQBYPrHuQMJwyCBlwB/////wLzBgMWAf9v////AAZnA/8f/////////wT0BgMpAQCTCP8f////AQIZBgVx/////wr0BwYlAAJkAAZnCwlzCP8f/wPxAgcjCgyFCwkUAwBxBP8vCgxjDQYjAwKiBQkSDxc6/////wPxBgtEDQ9S/wjyBQEz/////xD1DAtZBwRkDwkUBQZxBww1EQ1hFQsVBgdTChBaEg5BBxElExVz/w/yCQtRChA4EhMhEQ0VCwxhDREmFf9P////CAky/////xb0GhI2DAqlFQ0lCw5hChJTExolChAWGRyZExUlDgcmFQ1HEQ4hEhYqGRShEhYYGRyIGhUlDROB////Dw1DFBpXF/8vGRIZEP9P/////xjxFBokG/9v////FQ0l////////HBkhFBaRHBQYEhaRGP8f////Gf9vHBtj/xf0DRSiHP8v////////Fxpj////////GxcpGhlhAAQABwAEAACaITcmQA0SBZ2xZaAFGBGBtIUgDjMIpcT24BAqA75EBgEFLQt6uR0hBSAOfcQ5gQxHCpTFQcEOHwSr1mbhAxYOedF1AQc9DnnJfmETOQKuU4FhDxIHqVWKwQ4kCqRhxQEKNQaD2O0BCjUHhF39QQ4nC5vMBiIPMQee4gqiBT4LcssdAhYxArdfPcINLBSW0EViECYIoF51wg4YE5jMloIPGA2ac7qCBicJh026ghchA6zoEuMGJAmIzBnDFhYFpFs6YxUeCJvjRYMMOASK05njExQGhWWlQxMcCIT2+kMGEAeG6RpkDSkJgowBBgEY/////////wLx////AAaGBP8f////AP8f/wP0BgQZAf+P/////wr1BwYlAQLECP8f////AQIZBgVxBAIYBgliCP8f////AgMVBw8kDQkTBf9vA/8vCgtvDQklBgIhAgmCERdI/////wXxAgZTDREy/wjyBQEi/////xL1EAtPBwNlDAn/Bgf//wr/Eg//DQk2BgcxCwr2Eg+hEQkTBQZhDA80DhcUDA8jExdD/xHyCQ1BFw4TBgxBChBRFBMhChJIFBUhEw8RDQxiDhMmF/9f////CAlC/////xj0HBQlCwr1Fw4kDQ9RChRSFRwUChIVGBaRFRMSEAwkFxFIExARFBgaFhwSFBgZGx2fHBcmFRAS////EQ5TFRxHGf8/GxYZFBKU/////xrxFRwUH/9/////FxMx////////GxwWFhiRIBwmFhiRGv8f/x3/Gx5vIB9j/xn0DhaSG///////Hhz/FhT/IBz/Fhv/Hf//////IP8/////////GRxzHv//////Hxk6HBthpw5F+uAQEwm9wz1hDEIOscxZIRMiA8FYjuEOIwu8056hBjIIj8z6IQ8tCbJfEQIOJA+p4h7iBDYIil9SAg4hD6rQUqIPIAmz5wGjBiUJpOJBoww0BaVnqWMTGwqW6hoEDScKnqgAAwEU/////////wLz/wD1AwU1BwQT/////////wz6BQM1AP8/BwQ1AQAxAv9fDAXhAQM1Bgdx////////Av8//wnxBgcVBANxCgQXAQNRBf8fCQghBghWCv9v/////wTxCgQYAQZR/wnxDAu0Av8f/wvzCgghBgUhCQslDf+v////Bwhh/wz3Df9v/wr1Bwi0DQsXCf+v////////DP8f/////wr6CwJqhxPBAYEOEAe8SAoBERQJwcUpgQxCDbPFSYETGQXA0FnhAg8UetCGIQcyDJNMhgEVCQO8WZahDiMMucvqYQ8uCLbhDmIFOQmLYSGCDSwQp88+4g8iBbZhYqINGg2o5QEDByUJpeExAw00BaZVRaMVFQmu1Y1DFBMKmmixAxMbCpfpEqQNKgid5AD///8BB/8KAv////8HAC////////8DCzL/AP8DB3MJBRP/////////BvIIBzUB/z//Bf8KCf////////8CBzYKDXgJBC////8IB1cD/y//////D/8JBVYCAD8DBlcICiEDBjX/C/IKCRYFB4IHClUN/2////8EBfL/BfgCB0EICxIMDhUG/z8PEP8MCiIFCMINCRcKCBELDy8QDvQMDhQS/6////8JCmH/EfYS/2//DfQJDLQQDv8LBv////////8P//////8RDv8LBv8SDhYMEL////////8R/x//////DfoOD2+wErdJwAoeBIOsiqAGHA94u5kgDjQHjE3qYAUuB3jFFQERLQOdxlFBDEcLfNeJYQY3CWLGnkETMgWPWb1BCjUHcdb9oQk0B2vjCcIELA5nzTnCFTIDlVKlghcjA5BwsgIHKAlwcFaDChYIeuRaYwwoB3bxbQMIFAZ7aImDDRYHcdgA/////wL/BQH/////////AAX2BgMh/////////wT1BQMpAQCP////////AQIZBQZz/////wf0CQVWAAL1AgQmBw6aCAYUAwB/BQhECQpS/////wPz/////wv1DwhLBQSUCgYkAwVxBAdrEQnhBwuuEQ3T/wrzBghRCQs+Df9f/////wby////DP9PDwk+BQflEQleC/9P////////////CglTCw7GEP9vEA0WCQuUDxET////DP9fEf8vEA4hCQujDv8f////////DQxoEA9CCQzW////////1RK4iSAOMwiMSvpABSwFe8UJIREsA5/IOeEEHhB7xUGBDEcIf9J94QY4DWPIjkETNwWQYMnhCTYHcNnx4Qk0CG/hDSIFLg5nzCniFTQCmVKxYhcjBJRyusIGKApz5/1CByQIcuZOwwwrBnh3XkMKFgd782ljCBUGfG2ZQw0WB3DYAP////8C9AQBGf////////////8A+QQDf/////8G9AcEVf8A9P8E/wUJ//////8B/wACFQYOmwcFEwH/fwAEUwcJMf///wP///////8K9Q4HWwQClAkFEwEEcQIKXg4IsQYKrQ4Mown/LwUHQQgKLgz/X////wMF8f////8L8w4ILQQG1Q4IXgYKk////////////wkIUwoPxw3//woP/xD//////wwI/wv/XxH/Lw8NLwgKohANHwgLlw7/L////w//H////////w0L9xAPMw4LI////////w==</t>
-  </si>
-  <si>
     <t>CECEP4224</t>
   </si>
   <si>
     <t>MULYANI4504</t>
   </si>
   <si>
-    <t>RUSTY3694</t>
-  </si>
-  <si>
     <t>NURLELA4298</t>
   </si>
   <si>
@@ -250,24 +211,15 @@
     <t>TIURLAN3947</t>
   </si>
   <si>
-    <t>EKO4670</t>
-  </si>
-  <si>
     <t>ANGGIA13424</t>
   </si>
   <si>
     <t>SRI4014</t>
   </si>
   <si>
-    <t>Frisilia4015</t>
-  </si>
-  <si>
     <t>MUHAMMAD16027</t>
   </si>
   <si>
-    <t>RARA41</t>
-  </si>
-  <si>
     <t>UserLDAP</t>
   </si>
   <si>
@@ -301,24 +253,6 @@
     <t>PAY002</t>
   </si>
   <si>
-    <t>GHI111222333</t>
-  </si>
-  <si>
-    <t>ADM1122334</t>
-  </si>
-  <si>
-    <t>TOPUP1</t>
-  </si>
-  <si>
-    <t>JKL444555666</t>
-  </si>
-  <si>
-    <t>SUP4455667</t>
-  </si>
-  <si>
-    <t>INV003</t>
-  </si>
-  <si>
     <t>MNO777888999</t>
   </si>
   <si>
@@ -355,15 +289,6 @@
     <t>INV007</t>
   </si>
   <si>
-    <t>YZA321654987</t>
-  </si>
-  <si>
-    <t>ADM3216549</t>
-  </si>
-  <si>
-    <t>SRV008</t>
-  </si>
-  <si>
     <t>BCD654321789</t>
   </si>
   <si>
@@ -436,27 +361,12 @@
     <t>SRV016</t>
   </si>
   <si>
-    <t>ZAB852741963</t>
-  </si>
-  <si>
-    <t>ADM8527419</t>
-  </si>
-  <si>
-    <t>PAY017</t>
-  </si>
-  <si>
     <t>00000000000000100000</t>
   </si>
   <si>
     <t>00000000000000250000</t>
   </si>
   <si>
-    <t>00000000000000075000</t>
-  </si>
-  <si>
-    <t>00000000000001000000</t>
-  </si>
-  <si>
     <t>00000000000000050000</t>
   </si>
   <si>
@@ -469,9 +379,6 @@
     <t>00000000000000120000</t>
   </si>
   <si>
-    <t>00000000000000030000</t>
-  </si>
-  <si>
     <t>00000000000000400000</t>
   </si>
   <si>
@@ -494,9 +401,6 @@
   </si>
   <si>
     <t>00000000000000180000</t>
-  </si>
-  <si>
-    <t>00000000000000099000</t>
   </si>
 </sst>
 </file>
@@ -860,10 +764,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -891,19 +795,19 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="F1" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="G1" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="H1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="I1" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="J1" t="s">
         <v>4</v>
@@ -923,19 +827,19 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>141</v>
+        <v>113</v>
       </c>
       <c r="J2" t="s">
         <v>8</v>
@@ -955,19 +859,19 @@
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>142</v>
+        <v>114</v>
       </c>
       <c r="J3" t="s">
         <v>11</v>
@@ -975,31 +879,31 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>3694</v>
+        <v>3947</v>
       </c>
       <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
       <c r="E4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>143</v>
+        <v>115</v>
       </c>
       <c r="J4" t="s">
         <v>15</v>
@@ -1007,7 +911,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>4670</v>
+        <v>4298</v>
       </c>
       <c r="B5" t="s">
         <v>16</v>
@@ -1016,246 +920,246 @@
         <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="J5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>3947</v>
+        <v>13424</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>145</v>
+        <v>117</v>
       </c>
       <c r="J6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>4298</v>
+        <v>4014</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E7" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
       <c r="J7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>13424</v>
+        <v>20153</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E8" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>147</v>
+        <v>119</v>
       </c>
       <c r="J8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>4014</v>
+        <v>6735</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E9" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>148</v>
+        <v>120</v>
       </c>
       <c r="J9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>4015</v>
+        <v>16027</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E10" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>149</v>
+        <v>121</v>
       </c>
       <c r="J10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>20153</v>
+        <v>20703</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E11" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>150</v>
+        <v>122</v>
       </c>
       <c r="J11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>6735</v>
+        <v>9790</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D12" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="J12" t="s">
         <v>42</v>
@@ -1263,63 +1167,63 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>16027</v>
+        <v>1234567</v>
       </c>
       <c r="B13" t="s">
         <v>43</v>
       </c>
       <c r="C13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="J13" t="s">
         <v>44</v>
-      </c>
-      <c r="D13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" t="s">
-        <v>80</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="J13" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>20703</v>
+        <v>30</v>
       </c>
       <c r="B14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" t="s">
         <v>46</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>47</v>
       </c>
-      <c r="D14" t="s">
-        <v>41</v>
-      </c>
       <c r="E14" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="H14" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I14" s="2" t="s">
         <v>125</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>153</v>
       </c>
       <c r="J14" t="s">
         <v>48</v>
@@ -1327,7 +1231,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>9790</v>
+        <v>40</v>
       </c>
       <c r="B15" t="s">
         <v>49</v>
@@ -1336,153 +1240,25 @@
         <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="E15" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="F15" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="I15" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>154</v>
-      </c>
       <c r="J15" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>1234567</v>
-      </c>
-      <c r="B16" t="s">
         <v>52</v>
-      </c>
-      <c r="C16" t="s">
-        <v>52</v>
-      </c>
-      <c r="D16" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" t="s">
-        <v>52</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="J16" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>30</v>
-      </c>
-      <c r="B17" t="s">
-        <v>54</v>
-      </c>
-      <c r="C17" t="s">
-        <v>55</v>
-      </c>
-      <c r="D17" t="s">
-        <v>56</v>
-      </c>
-      <c r="E17" t="s">
-        <v>73</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="J17" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>40</v>
-      </c>
-      <c r="B18" t="s">
-        <v>58</v>
-      </c>
-      <c r="C18" t="s">
-        <v>59</v>
-      </c>
-      <c r="D18" t="s">
-        <v>60</v>
-      </c>
-      <c r="E18" t="s">
-        <v>74</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="J18" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>41</v>
-      </c>
-      <c r="B19" t="s">
-        <v>62</v>
-      </c>
-      <c r="C19" t="s">
-        <v>63</v>
-      </c>
-      <c r="D19" t="s">
-        <v>60</v>
-      </c>
-      <c r="E19" t="s">
-        <v>81</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="J19" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>